<commit_message>
backup before new cor_and_elas extended
</commit_message>
<xml_diff>
--- a/fourth_pass/welfare_results/3282/analysis_results/cor_and_elas_extended_3282.xlsx
+++ b/fourth_pass/welfare_results/3282/analysis_results/cor_and_elas_extended_3282.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t xml:space="preserve">tot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tot_excl</t>
   </si>
   <si>
     <t xml:space="preserve">w</t>
@@ -449,46 +452,46 @@
         <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>0.966114154821934</v>
+        <v>0.966114154743509</v>
       </c>
       <c r="C2" t="n">
-        <v>189.172470588797</v>
+        <v>189.172470010823</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.972262885184565</v>
+        <v>-0.972262885185545</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.968406992009873</v>
+        <v>-0.968406992011181</v>
       </c>
       <c r="F2" t="n">
-        <v>0.965572319977136</v>
+        <v>0.96557232001688</v>
       </c>
       <c r="G2" t="n">
-        <v>-12.417996289589</v>
+        <v>-12.4179962894858</v>
       </c>
       <c r="H2" t="n">
-        <v>-676.715798029307</v>
+        <v>-676.715798022042</v>
       </c>
       <c r="I2" t="n">
-        <v>3.45568157505463</v>
+        <v>3.4556815671311</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.443910646922249</v>
+        <v>-0.443910646922209</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.490921519323632</v>
+        <v>-0.4909215193235</v>
       </c>
       <c r="L2" t="n">
-        <v>0.965572319977136</v>
+        <v>0.96557232001688</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.0238422095945621</v>
+        <v>-0.0238422095946534</v>
       </c>
       <c r="N2" t="n">
-        <v>-1.44259223513687</v>
+        <v>-1.44259223514332</v>
       </c>
       <c r="O2" t="n">
-        <v>3.45568157505463</v>
+        <v>3.4556815671311</v>
       </c>
     </row>
     <row r="3">
@@ -496,46 +499,46 @@
         <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.547610477341699</v>
+        <v>0.966114154821934</v>
       </c>
       <c r="C3" t="n">
-        <v>-8.03788522848991</v>
+        <v>189.172470588797</v>
       </c>
       <c r="D3" t="n">
-        <v>0.961595440583135</v>
+        <v>-0.972262885184565</v>
       </c>
       <c r="E3" t="n">
-        <v>0.957350573531521</v>
+        <v>-0.968406992009873</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.670866990971024</v>
+        <v>0.965572319977136</v>
       </c>
       <c r="G3" t="n">
-        <v>0.46888338418371</v>
+        <v>-12.417996289589</v>
       </c>
       <c r="H3" t="n">
-        <v>25.5401844753712</v>
+        <v>-676.715798029307</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.179980682717625</v>
+        <v>3.45568157505463</v>
       </c>
       <c r="J3" t="n">
-        <v>0.962560466016621</v>
+        <v>-0.443910646922249</v>
       </c>
       <c r="K3" t="n">
-        <v>0.96027381548227</v>
+        <v>-0.490921519323632</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.670866990971024</v>
+        <v>0.965572319977136</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0369247801650946</v>
+        <v>-0.0238422095945621</v>
       </c>
       <c r="N3" t="n">
-        <v>2.01542000583736</v>
+        <v>-1.44259223513687</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.179980682717625</v>
+        <v>3.45568157505463</v>
       </c>
     </row>
     <row r="4">
@@ -543,45 +546,92 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
+        <v>-0.547610477356539</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-8.03788502365533</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.961595440589842</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.957350573531041</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.670866991702172</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.468883384034928</v>
+      </c>
+      <c r="H4" t="n">
+        <v>25.5401844642189</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-0.179980680400155</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.962560466016732</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.960273815482235</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.670866991702172</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0369247801652082</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2.01542000584516</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.179980680400155</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.968730928781065</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>197.210355817287</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>-0.974804239306992</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E5" t="n">
         <v>-0.970922359911934</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F5" t="n">
         <v>0.977096733395536</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G5" t="n">
         <v>-12.8868796737727</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H5" t="n">
         <v>-702.255982504678</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I5" t="n">
         <v>3.63566225777225</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J5" t="n">
         <v>-0.827601642667028</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K5" t="n">
         <v>-0.860794665039772</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L5" t="n">
         <v>0.977096733395536</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M5" t="n">
         <v>-0.0607669897596567</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N5" t="n">
         <v>-3.45801224097423</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O5" t="n">
         <v>3.63566225777225</v>
       </c>
     </row>

</xml_diff>

<commit_message>
backup before fixing extend_animal_trends
</commit_message>
<xml_diff>
--- a/fourth_pass/welfare_results/3282/analysis_results/cor_and_elas_extended_3282.xlsx
+++ b/fourth_pass/welfare_results/3282/analysis_results/cor_and_elas_extended_3282.xlsx
@@ -452,46 +452,46 @@
         <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.999490387984652</v>
+        <v>-0.999391737847945</v>
       </c>
       <c r="C2" t="n">
-        <v>-167965945.557761</v>
+        <v>-168212921.728772</v>
       </c>
       <c r="D2" t="n">
-        <v>0.956625068060372</v>
+        <v>0.962855769528591</v>
       </c>
       <c r="E2" t="n">
-        <v>0.999490018715337</v>
+        <v>0.999391280599276</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.956629251004605</v>
+        <v>-0.962861929841827</v>
       </c>
       <c r="G2" t="n">
-        <v>123400.043840362</v>
+        <v>137191.16226133</v>
       </c>
       <c r="H2" t="n">
-        <v>7053953.60237105</v>
+        <v>7064317.99834326</v>
       </c>
       <c r="I2" t="n">
-        <v>-2938364.66570834</v>
+        <v>-3266764.51060286</v>
       </c>
       <c r="J2" t="n">
-        <v>0.958218396245853</v>
+        <v>0.963938592567792</v>
       </c>
       <c r="K2" t="n">
-        <v>0.999569298810958</v>
+        <v>0.999483086929724</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.956629251004605</v>
+        <v>-0.962861929841827</v>
       </c>
       <c r="M2" t="n">
-        <v>51.2251243362736</v>
+        <v>56.8097427097398</v>
       </c>
       <c r="N2" t="n">
-        <v>2923.55996441976</v>
+        <v>2922.25889993025</v>
       </c>
       <c r="O2" t="n">
-        <v>-2938364.66570834</v>
+        <v>-3266764.51060286</v>
       </c>
     </row>
     <row r="3">
@@ -499,46 +499,46 @@
         <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>0.966114154821934</v>
+        <v>0.960692208521904</v>
       </c>
       <c r="C3" t="n">
-        <v>189.172470588797</v>
+        <v>191.766895909241</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.972262885184565</v>
+        <v>-0.989801480892533</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.968406992009873</v>
+        <v>-0.962466664394755</v>
       </c>
       <c r="F3" t="n">
-        <v>0.965572319977136</v>
+        <v>0.985316499870559</v>
       </c>
       <c r="G3" t="n">
-        <v>-12.417996289589</v>
+        <v>-14.1145160291415</v>
       </c>
       <c r="H3" t="n">
-        <v>-676.715798029307</v>
+        <v>-680.884385471807</v>
       </c>
       <c r="I3" t="n">
-        <v>3.45568157505463</v>
+        <v>3.96456314240996</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.443910646922249</v>
+        <v>-0.941145086554243</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.490921519323632</v>
+        <v>-0.83308458247653</v>
       </c>
       <c r="L3" t="n">
-        <v>0.965572319977136</v>
+        <v>0.985316499870559</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.0238422095945621</v>
+        <v>-0.055190831530792</v>
       </c>
       <c r="N3" t="n">
-        <v>-1.44259223513687</v>
+        <v>-2.42364630721163</v>
       </c>
       <c r="O3" t="n">
-        <v>3.45568157505463</v>
+        <v>3.96456314240996</v>
       </c>
     </row>
     <row r="4">
@@ -546,46 +546,46 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.999490392340614</v>
+        <v>-0.999391742941703</v>
       </c>
       <c r="C4" t="n">
-        <v>-167966143.768117</v>
+        <v>-168213116.810482</v>
       </c>
       <c r="D4" t="n">
-        <v>0.956629474753855</v>
+        <v>0.962861972874171</v>
       </c>
       <c r="E4" t="n">
-        <v>0.999490393066385</v>
+        <v>0.999391739254949</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.956629315659008</v>
+        <v>-0.962862005314365</v>
       </c>
       <c r="G4" t="n">
-        <v>123411.930720036</v>
+        <v>137204.700074537</v>
       </c>
       <c r="H4" t="n">
-        <v>7054603.24085416</v>
+        <v>7064972.81960954</v>
       </c>
       <c r="I4" t="n">
-        <v>-2938368.31894859</v>
+        <v>-3266768.53858099</v>
       </c>
       <c r="J4" t="n">
-        <v>0.956661154052383</v>
+        <v>0.962855643078381</v>
       </c>
       <c r="K4" t="n">
-        <v>0.999490528013075</v>
+        <v>0.999391020084426</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.956629315659008</v>
+        <v>-0.962862005314365</v>
       </c>
       <c r="M4" t="n">
-        <v>50.2858913260332</v>
+        <v>55.898545045192</v>
       </c>
       <c r="N4" t="n">
-        <v>2874.40047728179</v>
+        <v>2878.35630414182</v>
       </c>
       <c r="O4" t="n">
-        <v>-2938368.31894859</v>
+        <v>-3266768.53858099</v>
       </c>
     </row>
     <row r="5">
@@ -593,46 +593,46 @@
         <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>0.968730928781065</v>
+        <v>0.961809438901286</v>
       </c>
       <c r="C5" t="n">
-        <v>197.210355817287</v>
+        <v>194.081710310473</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.974804239306992</v>
+        <v>-0.990159378487734</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.970922359911934</v>
+        <v>-0.964998854783382</v>
       </c>
       <c r="F5" t="n">
-        <v>0.977096733395536</v>
+        <v>0.985485299274315</v>
       </c>
       <c r="G5" t="n">
-        <v>-12.8868796737727</v>
+        <v>-14.5378132072954</v>
       </c>
       <c r="H5" t="n">
-        <v>-702.255982504678</v>
+        <v>-702.895176981353</v>
       </c>
       <c r="I5" t="n">
-        <v>3.63566225777225</v>
+        <v>4.00844509920539</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.827601642667028</v>
+        <v>-0.994071220285752</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.860794665039772</v>
+        <v>-0.941231183566587</v>
       </c>
       <c r="L5" t="n">
-        <v>0.977096733395536</v>
+        <v>0.985485299274315</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.0607669897596567</v>
+        <v>-0.0888023354520817</v>
       </c>
       <c r="N5" t="n">
-        <v>-3.45801224097423</v>
+        <v>-4.17131493677733</v>
       </c>
       <c r="O5" t="n">
-        <v>3.63566225777225</v>
+        <v>4.00844509920539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
backup before stacking population plots four panel
</commit_message>
<xml_diff>
--- a/fourth_pass/welfare_results/3282/analysis_results/cor_and_elas_extended_3282.xlsx
+++ b/fourth_pass/welfare_results/3282/analysis_results/cor_and_elas_extended_3282.xlsx
@@ -452,46 +452,46 @@
         <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.999490387148179</v>
+        <v>-0.999490387077816</v>
       </c>
       <c r="C2" t="n">
-        <v>-167965927.894281</v>
+        <v>-167965926.03901</v>
       </c>
       <c r="D2" t="n">
-        <v>0.956622052075795</v>
+        <v>0.956621583642287</v>
       </c>
       <c r="E2" t="n">
-        <v>0.999489957195813</v>
+        <v>0.999489950006617</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.956629209929808</v>
+        <v>-0.956629205321652</v>
       </c>
       <c r="G2" t="n">
-        <v>123398.709589424</v>
+        <v>123398.51151122</v>
       </c>
       <c r="H2" t="n">
-        <v>7053899.13708228</v>
+        <v>7053891.21761726</v>
       </c>
       <c r="I2" t="n">
-        <v>-2938364.23300129</v>
+        <v>-2938364.18659807</v>
       </c>
       <c r="J2" t="n">
-        <v>0.958059008831814</v>
+        <v>0.958038616411136</v>
       </c>
       <c r="K2" t="n">
-        <v>0.999569290816084</v>
+        <v>0.999569340352638</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.956629209929808</v>
+        <v>-0.956629205321652</v>
       </c>
       <c r="M2" t="n">
-        <v>51.1952158054426</v>
+        <v>51.191570113583</v>
       </c>
       <c r="N2" t="n">
-        <v>2922.33907206554</v>
+        <v>2922.19331181278</v>
       </c>
       <c r="O2" t="n">
-        <v>-2938364.23300129</v>
+        <v>-2938364.18659807</v>
       </c>
     </row>
     <row r="3">
@@ -499,46 +499,46 @@
         <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>0.96075179708399</v>
+        <v>0.958630856791998</v>
       </c>
       <c r="C3" t="n">
-        <v>206.835950169165</v>
+        <v>208.691221224262</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.990918287884244</v>
+        <v>-0.99186416443196</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.962960650780198</v>
+        <v>-0.960485486419506</v>
       </c>
       <c r="F3" t="n">
-        <v>0.988178552750225</v>
+        <v>0.988893602938317</v>
       </c>
       <c r="G3" t="n">
-        <v>-13.7522472273616</v>
+        <v>-13.9503254317761</v>
       </c>
       <c r="H3" t="n">
-        <v>-731.181086803771</v>
+        <v>-739.100551819794</v>
       </c>
       <c r="I3" t="n">
-        <v>3.88838862067452</v>
+        <v>3.93479185101298</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.954709345381321</v>
+        <v>-0.959852434254271</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.864681824892635</v>
+        <v>-0.858674536582941</v>
       </c>
       <c r="L3" t="n">
-        <v>0.988178552750225</v>
+        <v>0.988893602938317</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.0537507404254872</v>
+        <v>-0.057396432285014</v>
       </c>
       <c r="N3" t="n">
-        <v>-2.66348458934856</v>
+        <v>-2.80924484210361</v>
       </c>
       <c r="O3" t="n">
-        <v>3.88838862067452</v>
+        <v>3.93479185101298</v>
       </c>
     </row>
     <row r="4">
@@ -593,46 +593,46 @@
         <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>0.96180749989664</v>
+        <v>0.959724684595245</v>
       </c>
       <c r="C5" t="n">
-        <v>209.082491389357</v>
+        <v>210.937762444454</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.99100676797505</v>
+        <v>-0.992003284461223</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.965298129808319</v>
+        <v>-0.962931925400802</v>
       </c>
       <c r="F5" t="n">
-        <v>0.988226198770939</v>
+        <v>0.988964243022986</v>
       </c>
       <c r="G5" t="n">
-        <v>-14.1283462427936</v>
+        <v>-14.326424447208</v>
       </c>
       <c r="H5" t="n">
-        <v>-752.933732297715</v>
+        <v>-760.853197313738</v>
       </c>
       <c r="I5" t="n">
-        <v>3.92649717991856</v>
+        <v>3.97290041025702</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.990251794262538</v>
+        <v>-0.994758130049207</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.950411360499961</v>
+        <v>-0.945219214524355</v>
       </c>
       <c r="L5" t="n">
-        <v>0.988226198770939</v>
+        <v>0.988964243022986</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.083616573730455</v>
+        <v>-0.0872622655899818</v>
       </c>
       <c r="N5" t="n">
-        <v>-4.39075221822583</v>
+        <v>-4.53651247098088</v>
       </c>
       <c r="O5" t="n">
-        <v>3.92649717991856</v>
+        <v>3.97290041025702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>